<commit_message>
- Actualizacion de templates y agregar Plantilla de formato de JAM
</commit_message>
<xml_diff>
--- a/Template/Export/MuestrasLab_17.xlsx
+++ b/Template/Export/MuestrasLab_17.xlsx
@@ -68,9 +68,6 @@
     <t>Date Shipped</t>
   </si>
   <si>
-    <t>NATIONAL PUBLIC HEALTH LABORATORY</t>
-  </si>
-  <si>
     <t>21 Slipe Pen Road
 Kingston Jamaica</t>
   </si>
@@ -172,6 +169,9 @@
       </rPr>
       <t>:</t>
     </r>
+  </si>
+  <si>
+    <t>LINE LISTING OF SAMPLES SENT TO NIC BY NPHL</t>
   </si>
 </sst>
 </file>
@@ -275,23 +275,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,62 +614,62 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:N1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="20" style="12" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="13" style="14" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="12" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" style="12" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" style="14" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" style="14" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="20" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="13" style="12" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" style="10" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="12" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
+      <c r="A1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
+      <c r="A2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" spans="1:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3"/>
@@ -689,7 +689,7 @@
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="3"/>
@@ -702,14 +702,14 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="3"/>
@@ -722,17 +722,17 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -744,17 +744,17 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>

</xml_diff>